<commit_message>
Archivos clase viernes 1 de octubre
</commit_message>
<xml_diff>
--- a/Carga masiva.xlsx
+++ b/Carga masiva.xlsx
@@ -5,13 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="regiones" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="comunas" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="empleados" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="roles" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="usuarios" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="ventas" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="clientes" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="92">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -127,6 +130,9 @@
     <t xml:space="preserve">rol_id</t>
   </si>
   <si>
+    <t xml:space="preserve">Empleado Rol</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comuna</t>
   </si>
   <si>
@@ -182,21 +188,155 @@
   </si>
   <si>
     <t xml:space="preserve">karen.jara@hotmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empleado_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empleado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javiera Gonzalez - Administrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kjara.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karen Jara - Vendedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lperez.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luis Perez - Vendedor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fecha_hora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usuario_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cliente_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Query</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">empresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empresa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opcion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18890300-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noemi Caceres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ncaceres@movistar.cl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96983012-K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alarcon SA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jalarcon@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Los Pinguinos 444</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10982700-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Productos del Mar SpA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">m.morales@hotmail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.com</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Arturo Prat 1245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15632902-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samuel Vergara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svergara@yahoo.es</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16789564-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paula Ramirez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paula.ramirez@aiep.cl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -218,6 +358,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -268,7 +409,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,11 +426,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -313,10 +462,10 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="L3:L4 D2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="K4:K6 D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="58.4"/>
@@ -595,13 +744,13 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="L3:L4 F2"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="1" sqref="K4:K6 F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="57.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,7 +944,7 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -808,16 +957,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3:L4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="K4:K6 I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="149.55"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="149.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -845,13 +995,20 @@
       <c r="H1" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="0" t="str">
+        <f aca="false">A1</f>
+        <v>id</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -860,117 +1017,155 @@
         <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" s="0" t="n">
-        <f aca="false">VLOOKUP(I2,comunas!B:E,4,0)</f>
+        <f aca="false">VLOOKUP(K2,comunas!B:E,4,0)</f>
         <v>4</v>
       </c>
       <c r="H2" s="0" t="n">
-        <f aca="false">VLOOKUP(J2,roles!B:C,2,0)</f>
+        <f aca="false">VLOOKUP(L2,roles!B:C,2,0)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="4" t="str">
+        <f aca="false">_xlfn.CONCAT(C2," - ",L2)</f>
+        <v>Javiera Gonzalez - Administrador</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <f aca="false">A2</f>
+        <v>2</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="0" t="str">
+      <c r="L2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO empleados(rut, nombre, fecha_nac, direccion, email, comuna_id, rol_id) VALUES('",B2,"', '",C2,"', ",D2,", '",E2,"', '",F2,"', ",G2,", ",H2,");")</f>
         <v>INSERT INTO empleados(rut, nombre, fecha_nac, direccion, email, comuna_id, rol_id) VALUES('20900600-3', 'Javiera Gonzalez', '2001-02-15', 'Argomedo 102', 'jgonzalez@gmail.com', 4, 1);</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="B3" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="F3" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="G3" s="0" t="n">
-        <f aca="false">VLOOKUP(I3,comunas!B:E,4,0)</f>
+        <f aca="false">VLOOKUP(K3,comunas!B:E,4,0)</f>
         <v>8</v>
       </c>
       <c r="H3" s="0" t="n">
-        <f aca="false">VLOOKUP(J3,roles!B:C,2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="I3" s="4" t="s">
+        <f aca="false">VLOOKUP(L3,roles!B:C,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT(C3," - ",L3)</f>
+        <v>Luis Perez - Vendedor</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <f aca="false">A3</f>
+        <v>4</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="0" t="str">
+      <c r="L3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO empleados(rut, nombre, fecha_nac, direccion, email, comuna_id, rol_id) VALUES('",B3,"', '",C3,"', ",D3,", '",E3,"', '",F3,"', ",G3,", ",H3,");")</f>
         <v>INSERT INTO empleados(rut, nombre, fecha_nac, direccion, email, comuna_id, rol_id) VALUES('14632870-K', 'Luis Perez', '1978-10-22', 'San Martin 888', 'lperez@gmail.com', 8, 2);</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>5</v>
+      </c>
       <c r="B4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">VLOOKUP(K4,comunas!B:E,4,0)</f>
+        <v>6</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">VLOOKUP(L4,roles!B:C,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT(C4," - ",L4)</f>
+        <v>Karen Jara - Vendedor</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>5</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <f aca="false">VLOOKUP(I4,comunas!B:E,4,0)</f>
-        <v>6</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <f aca="false">VLOOKUP(J4,roles!B:C,2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L4" s="0" t="str">
+      <c r="N4" s="0" t="str">
         <f aca="false">_xlfn.CONCAT("INSERT INTO empleados(rut, nombre, fecha_nac, direccion, email, comuna_id, rol_id) VALUES('",B4,"', '",C4,"', ",D4,", '",E4,"', '",F4,"', ",G4,", ",H4,");")</f>
         <v>INSERT INTO empleados(rut, nombre, fecha_nac, direccion, email, comuna_id, rol_id) VALUES('18745600-1', 'Karen Jara', '1995-03-05', 'Carrera 349', 'karen.jara@hotmail.com', 6, 2);</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I4" type="list">
+  <dataValidations count="4">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K2:K4" type="list">
       <formula1>comunas!$B$2:$B$40</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J4" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2:L4" type="list">
       <formula1>roles!$B$2:$B$10</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2" type="list">
+      <formula1>empleados!$M$2:$M$20</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I3" type="list">
+      <formula1>empleados!$I$2:$I$20</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -980,7 +1175,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -996,10 +1191,10 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="L3:L4 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="K4:K6 C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1008,7 +1203,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="str">
+      <c r="C1" s="7" t="str">
         <f aca="false">A1</f>
         <v>id</v>
       </c>
@@ -1018,7 +1213,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">A2</f>
@@ -1030,7 +1225,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" s="0" t="n">
         <f aca="false">A3</f>
@@ -1046,7 +1241,1057 @@
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="K4:K6 A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="67.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="0" t="str">
+        <f aca="false">A1</f>
+        <v>id</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>123456</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <f aca="false">VLOOKUP(E2,empleados!I:J,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="G2" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO usuarios(clave,activo,empleado_id) VALUES(sha1('",B2,"'), ",C2,", ",D2,");")</f>
+        <v>INSERT INTO usuarios(clave,activo,empleado_id) VALUES(sha1('123456'), 1, 2);</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <f aca="false">VLOOKUP(E3,empleados!I:J,2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <f aca="false">A3</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO usuarios(clave,activo,empleado_id) VALUES(sha1('",B3,"'), ",C3,", ",D3,");")</f>
+        <v>INSERT INTO usuarios(clave,activo,empleado_id) VALUES(sha1('Kjara.123'), 1, 5);</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <f aca="false">VLOOKUP(E4,empleados!I:J,2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO usuarios(clave,activo,empleado_id) VALUES(sha1('",B4,"'), ",C4,", ",D4,");")</f>
+        <v>INSERT INTO usuarios(clave,activo,empleado_id) VALUES(sha1('Lperez.123'), 1, 4);</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E2:E4" type="list">
+      <formula1>empleados!$I$2:$I$20</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I3" activeCellId="1" sqref="K4:K6 I3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.23"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="0" t="str">
+        <f aca="false">A1</f>
+        <v>id</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <f aca="false">VLOOKUP(F2,usuarios!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C2,", ",D2,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),2, NULL);</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="n">
+        <f aca="false">VLOOKUP(F3,usuarios!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">A3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C3,", ",D3,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),2, NULL);</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C4" s="0" t="n">
+        <f aca="false">VLOOKUP(F4,usuarios!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C4,", ",D4,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),2, NULL);</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="0" t="n">
+        <f aca="false">VLOOKUP(F5,usuarios!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">A5</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C5,", ",D5,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),2, NULL);</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="0" t="n">
+        <f aca="false">VLOOKUP(F6,usuarios!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">A6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C6,", ",D6,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),2, NULL);</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C7" s="0" t="n">
+        <f aca="false">VLOOKUP(F7,usuarios!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <f aca="false">A7</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C7,", ",D7,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),2, NULL);</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="0" t="n">
+        <f aca="false">VLOOKUP(F8,usuarios!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <f aca="false">A8</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C8,", ",D8,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),2, NULL);</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="n">
+        <f aca="false">VLOOKUP(F9,usuarios!E:F,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <f aca="false">A9</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C9,", ",D9,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),2, NULL);</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0" t="n">
+        <f aca="false">VLOOKUP(F10,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <f aca="false">A10</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C10,", ",D10,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="0" t="n">
+        <f aca="false">VLOOKUP(F11,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <f aca="false">A11</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C11,", ",D11,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="0" t="n">
+        <f aca="false">VLOOKUP(F12,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <f aca="false">A12</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C12,", ",D12,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="n">
+        <f aca="false">VLOOKUP(F13,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <f aca="false">A13</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I13" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C13,", ",D13,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="0" t="n">
+        <f aca="false">VLOOKUP(F14,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <f aca="false">A14</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I14" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C14,", ",D14,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="n">
+        <f aca="false">VLOOKUP(F15,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">A15</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I15" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C15,", ",D15,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="0" t="n">
+        <f aca="false">VLOOKUP(F16,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <f aca="false">A16</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I16" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C16,", ",D16,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="0" t="n">
+        <f aca="false">VLOOKUP(F17,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <f aca="false">A17</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I17" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C17,", ",D17,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C18" s="0" t="n">
+        <f aca="false">VLOOKUP(F18,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <f aca="false">A18</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C18,", ",D18,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="n">
+        <f aca="false">VLOOKUP(F19,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <f aca="false">A19</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C19,", ",D19,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="0" t="n">
+        <f aca="false">VLOOKUP(F20,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <f aca="false">A20</f>
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C20,", ",D20,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="n">
+        <f aca="false">VLOOKUP(F21,usuarios!E:F,2,0)</f>
+        <v>3</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">A21</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="7" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),",C21,", ",D21,");")</f>
+        <v>INSERT INTO ventas(fecha_hora,usuario_id,cliente_id) VALUES(now(),3, NULL);</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F2:F21" type="list">
+      <formula1>usuarios!$E$2:$E$21</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4:K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="117.45"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="0" t="str">
+        <f aca="false">A1</f>
+        <v>id</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <f aca="false">VLOOKUP(I2,O:P,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">VLOOKUP(J2,comunas!B:E,4,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">A2</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B2,"', '",C2,"', '",D2,"', ",E2,", '",F2,"', ",G2,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('18890300-0', 'Noemi Caceres', 'ncaceres@movistar.cl', 2, '', 4);</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <f aca="false">VLOOKUP(I3,O:P,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">VLOOKUP(J3,comunas!B:E,4,0)</f>
+        <v>6</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">A3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B3,"', '",C3,"', '",D3,"', ",E3,", '",F3,"', ",G3,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('96983012-K', 'Alarcon SA', 'jalarcon@gmail.com', 1, 'Los Pinguinos 444', 6);</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <f aca="false">VLOOKUP(I4,O:P,2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">VLOOKUP(J4,comunas!B:E,4,0)</f>
+        <v>11</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">A4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B4,"', '",C4,"', '",D4,"', ",E4,", '",F4,"', ",G4,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('10982700-1', 'Productos del Mar SpA', 'm.morales@hotmail.com', 1, 'Arturo Prat 1245', 11);</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <f aca="false">VLOOKUP(I5,O:P,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">VLOOKUP(J5,comunas!B:E,4,0)</f>
+        <v>9</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">A5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B5,"', '",C5,"', '",D5,"', ",E5,", '",F5,"', ",G5,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('15632902-0', 'Samuel Vergara', 'svergara@yahoo.es', 2, '', 9);</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <f aca="false">VLOOKUP(I6,O:P,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">VLOOKUP(J6,comunas!B:E,4,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">A6</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B6,"', '",C6,"', '",D6,"', ",E6,", '",F6,"', ",G6,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('16789564-3', 'Paula Ramirez', 'paula.ramirez@aiep.cl', 2, '', 10);</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="0" t="n">
+        <f aca="false">A7</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B7,"', '",C7,"', '",D7,"', ",E7,", '",F7,"', ",G7,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="0" t="n">
+        <f aca="false">A8</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B8,"', '",C8,"', '",D8,"', ",E8,", '",F8,"', ",G8,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="0" t="n">
+        <f aca="false">A9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B9,"', '",C9,"', '",D9,"', ",E9,", '",F9,"', ",G9,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="0" t="n">
+        <f aca="false">A10</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B10,"', '",C10,"', '",D10,"', ",E10,", '",F10,"', ",G10,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="0" t="n">
+        <f aca="false">A11</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B11,"', '",C11,"', '",D11,"', ",E11,", '",F11,"', ",G11,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="0" t="n">
+        <f aca="false">A12</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B12,"', '",C12,"', '",D12,"', ",E12,", '",F12,"', ",G12,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="0" t="n">
+        <f aca="false">A13</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B13,"', '",C13,"', '",D13,"', ",E13,", '",F13,"', ",G13,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="0" t="n">
+        <f aca="false">A14</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B14,"', '",C14,"', '",D14,"', ",E14,", '",F14,"', ",G14,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="0" t="n">
+        <f aca="false">A15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B15,"', '",C15,"', '",D15,"', ",E15,", '",F15,"', ",G15,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H16" s="0" t="n">
+        <f aca="false">A16</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B16,"', '",C16,"', '",D16,"', ",E16,", '",F16,"', ",G16,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H17" s="0" t="n">
+        <f aca="false">A17</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B17,"', '",C17,"', '",D17,"', ",E17,", '",F17,"', ",G17,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="0" t="n">
+        <f aca="false">A18</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B18,"', '",C18,"', '",D18,"', ",E18,", '",F18,"', ",G18,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H19" s="0" t="n">
+        <f aca="false">A19</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B19,"', '",C19,"', '",D19,"', ",E19,", '",F19,"', ",G19,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H20" s="0" t="n">
+        <f aca="false">A20</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B20,"', '",C20,"', '",D20,"', ",E20,", '",F20,"', ",G20,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H21" s="0" t="n">
+        <f aca="false">A21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT("INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('",B21,"', '",C21,"', '",D21,"', ",E21,", '",F21,"', ",G21,");")</f>
+        <v>INSERT INTO clientes(rut,nombre,email,empresa,direccion,comuna_id) VALUES('', '', '', , '', );</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I2:I21" type="list">
+      <formula1>clientes!$O$2:$O$3</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2:J21" type="list">
+      <formula1>comunas!$B$2:$B$20</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="jalarcon@gmail.com"/>
+    <hyperlink ref="D4" r:id="rId2" display="m.morales@hotmail"/>
+    <hyperlink ref="D5" r:id="rId3" display="svergara@yahoo.es"/>
+    <hyperlink ref="D6" r:id="rId4" display="paula.ramirez@aiep.cl"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>